<commit_message>
convert 2000 and 2001 to 2007 HS
</commit_message>
<xml_diff>
--- a/docs/classificacao/Description_undergraduate.xlsx
+++ b/docs/classificacao/Description_undergraduate.xlsx
@@ -7,22 +7,23 @@
     <workbookView xWindow="360" yWindow="120" windowWidth="17115" windowHeight="12015"/>
   </bookViews>
   <sheets>
-    <sheet name="ID_course" sheetId="1" r:id="rId1"/>
+    <sheet name="CO_course" sheetId="1" r:id="rId1"/>
     <sheet name="Level" sheetId="2" r:id="rId2"/>
     <sheet name="Modality" sheetId="3" r:id="rId3"/>
     <sheet name="Adm_category" sheetId="4" r:id="rId4"/>
     <sheet name="Degree" sheetId="5" r:id="rId5"/>
     <sheet name="Academic_organization" sheetId="6" r:id="rId6"/>
+    <sheet name="Ethnicity" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ID_course!$A$1:$B$775</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CO_course!$A$1:$B$775</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1603" uniqueCount="1575">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1609" uniqueCount="1581">
   <si>
     <t>010B00</t>
   </si>
@@ -4623,9 +4624,6 @@
     <t>Formação militar</t>
   </si>
   <si>
-    <t>ID_Curso</t>
-  </si>
-  <si>
     <t>Nome Curso</t>
   </si>
   <si>
@@ -4686,18 +4684,6 @@
     <t>.</t>
   </si>
   <si>
-    <t>Universidade</t>
-  </si>
-  <si>
-    <t>Centro Universitário</t>
-  </si>
-  <si>
-    <t>Faculdade</t>
-  </si>
-  <si>
-    <t>Instituto Superior ou Escola Superior</t>
-  </si>
-  <si>
     <t>Bachelor</t>
   </si>
   <si>
@@ -4737,23 +4723,56 @@
     <t>Undergraduate</t>
   </si>
   <si>
-    <t>University</t>
-  </si>
-  <si>
-    <t>University Centre</t>
-  </si>
-  <si>
-    <t>Faculty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">High Education Institute or Higher School  </t>
+    <t>CO_Curso</t>
+  </si>
+  <si>
+    <t>Branca</t>
+  </si>
+  <si>
+    <t>Preta</t>
+  </si>
+  <si>
+    <t>Parda</t>
+  </si>
+  <si>
+    <t>Amarela</t>
+  </si>
+  <si>
+    <t>Não dispõe da informação</t>
+  </si>
+  <si>
+    <t>Não declarado</t>
+  </si>
+  <si>
+    <t>Indian</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>Asian</t>
+  </si>
+  <si>
+    <t>Multiracial </t>
+  </si>
+  <si>
+    <t>Unidentified</t>
+  </si>
+  <si>
+    <t>Unreported</t>
+  </si>
+  <si>
+    <t>Indígena</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -4792,6 +4811,12 @@
     <font>
       <sz val="9"/>
       <color rgb="FF242424"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -4849,7 +4874,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -4880,6 +4905,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -5267,13 +5307,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>1566</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>1533</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>1534</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>1535</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -12268,13 +12308,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
+        <v>1537</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>1538</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>1539</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>1540</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -12282,10 +12322,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>1536</v>
+        <v>1535</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>1570</v>
+        <v>1565</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -12293,10 +12333,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>1537</v>
+        <v>1536</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>1559</v>
+        <v>1554</v>
       </c>
     </row>
   </sheetData>
@@ -12309,7 +12349,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12322,13 +12362,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
+        <v>1537</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>1538</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="8" t="s">
         <v>1539</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>1540</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -12336,10 +12376,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>1541</v>
+        <v>1540</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>1541</v>
+        <v>1540</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -12347,10 +12387,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>1542</v>
+        <v>1541</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>1560</v>
+        <v>1555</v>
       </c>
     </row>
   </sheetData>
@@ -12376,13 +12416,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
+        <v>1537</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>1538</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="8" t="s">
         <v>1539</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>1540</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -12390,10 +12430,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>1561</v>
+        <v>1556</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -12401,10 +12441,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>1543</v>
+        <v>1542</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>1562</v>
+        <v>1557</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -12412,10 +12452,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>1544</v>
+        <v>1543</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>1563</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -12423,10 +12463,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>1545</v>
+        <v>1544</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>1564</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -12434,10 +12474,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>1565</v>
+        <v>1560</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -12445,10 +12485,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>1566</v>
+        <v>1561</v>
       </c>
     </row>
   </sheetData>
@@ -12476,13 +12516,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
+        <v>1537</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>1538</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="8" t="s">
         <v>1539</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>1540</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -12490,10 +12530,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>1558</v>
+        <v>1553</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -12501,10 +12541,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>1567</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -12512,21 +12552,21 @@
         <v>3</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>1568</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>1569</v>
+        <v>1564</v>
       </c>
     </row>
   </sheetData>
@@ -12537,10 +12577,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection sqref="A1:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12551,15 +12591,38 @@
     <col min="4" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="2.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37" style="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
+        <v>1537</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>1538</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="8" t="s">
         <v>1539</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>1540</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -12567,10 +12630,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>1554</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>1571</v>
+        <v>1567</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>1574</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -12578,10 +12641,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>1555</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>1572</v>
+        <v>1568</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>1575</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -12589,10 +12652,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>1556</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>1573</v>
+        <v>1569</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>1577</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -12600,14 +12663,44 @@
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>1557</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>1574</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9"/>
+        <v>1570</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>1576</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="10">
+        <v>5</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>1580</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>1573</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="10">
+        <v>6</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>1571</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>1578</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="10">
+        <v>0</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>1572</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>1579</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>